<commit_message>
testing desktop git setup
</commit_message>
<xml_diff>
--- a/Basic Arithmetic Exercise.xlsx
+++ b/Basic Arithmetic Exercise.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guru99-Jayesh\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8610"/>
   </bookViews>
@@ -56,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -109,13 +110,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,7 +424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -433,7 +435,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +476,7 @@
       <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <f>C2+D2</f>
         <v>16</v>
       </c>

</xml_diff>